<commit_message>
update excel, fix profile metric value is 0
</commit_message>
<xml_diff>
--- a/excel/all_datasets.xlsx
+++ b/excel/all_datasets.xlsx
@@ -1,15 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\Good Lab\overleaf\TC-Journal\data\TC_Log_result_processing\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CDF618-76A6-4695-968B-639018210B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -262,15 +280,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.000"/>
+    <numFmt numFmtId="176" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -285,6 +303,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -315,46 +340,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -365,10 +381,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -406,71 +422,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -498,7 +514,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -521,11 +537,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -534,13 +550,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -550,7 +566,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -559,7 +575,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -568,7 +584,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -576,10 +592,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -644,29 +660,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" style="7" width="18.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="9.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="14.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="10" width="26.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="10" width="24.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="10" width="26.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="10" width="24.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="9" width="34.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="18.375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.625" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.75" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.25" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -698,7 +716,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -712,7 +730,7 @@
         <v>1090108</v>
       </c>
       <c r="E2" s="6">
-        <v>6.693343239318574</v>
+        <v>6.6933432393185743</v>
       </c>
       <c r="F2" s="5">
         <v>487</v>
@@ -730,7 +748,7 @@
         <v>11.333227498528235</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -744,7 +762,7 @@
         <v>1049866</v>
       </c>
       <c r="E3" s="6">
-        <v>6.622089062697111</v>
+        <v>6.6220890626971114</v>
       </c>
       <c r="F3" s="5">
         <v>14</v>
@@ -759,10 +777,10 @@
         <v>977594</v>
       </c>
       <c r="J3" s="6">
-        <v>8.050491762716756</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+        <v>8.0504917627167565</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -794,7 +812,7 @@
         <v>12.836448536212412</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -823,10 +841,10 @@
         <v>1928091</v>
       </c>
       <c r="J5" s="6">
-        <v>4.503817435818375</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+        <v>4.5038174358183749</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -840,7 +858,7 @@
         <v>4659565</v>
       </c>
       <c r="E6" s="6">
-        <v>3.892076671044966</v>
+        <v>3.8920766710449661</v>
       </c>
       <c r="F6" s="5">
         <v>1411</v>
@@ -855,10 +873,10 @@
         <v>2888957</v>
       </c>
       <c r="J6" s="6">
-        <v>8.669311379419982</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+        <v>8.6693113794199821</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -872,7 +890,7 @@
         <v>5369472</v>
       </c>
       <c r="E7" s="6">
-        <v>8.771167627451717</v>
+        <v>8.7711676274517174</v>
       </c>
       <c r="F7" s="5">
         <v>4</v>
@@ -890,7 +908,7 @@
         <v>12.005670696569418</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -904,7 +922,7 @@
         <v>6649470</v>
       </c>
       <c r="E8" s="6">
-        <v>19.40799439604221</v>
+        <v>19.407994396042209</v>
       </c>
       <c r="F8" s="5">
         <v>1854</v>
@@ -922,7 +940,7 @@
         <v>21.00548105532981</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -936,7 +954,7 @@
         <v>11095298</v>
       </c>
       <c r="E9" s="6">
-        <v>13.08087702596358</v>
+        <v>13.080877025963581</v>
       </c>
       <c r="F9" s="5">
         <v>988</v>
@@ -954,7 +972,7 @@
         <v>15.070254968263445</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row r="10" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -968,7 +986,7 @@
         <v>16518947</v>
       </c>
       <c r="E10" s="6">
-        <v>8.752297889565664</v>
+        <v>8.7522978895656642</v>
       </c>
       <c r="F10" s="5">
         <v>0</v>
@@ -986,7 +1004,7 @@
         <v>10.693038853683564</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row r="11" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -1015,10 +1033,10 @@
         <v>22132301</v>
       </c>
       <c r="J11" s="6">
-        <v>30.2653391232169</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+        <v>30.265339123216901</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -1032,7 +1050,7 @@
         <v>28183518</v>
       </c>
       <c r="E12" s="6">
-        <v>21.66315689954216</v>
+        <v>21.663156899542159</v>
       </c>
       <c r="F12" s="5">
         <v>37378</v>
@@ -1050,7 +1068,7 @@
         <v>23.027554001277394</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row r="13" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
@@ -1064,7 +1082,7 @@
         <v>34681189</v>
       </c>
       <c r="E13" s="6">
-        <v>17.34943403664167</v>
+        <v>17.349434036641671</v>
       </c>
       <c r="F13" s="5">
         <v>9274</v>
@@ -1082,7 +1100,7 @@
         <v>20.777244616593066</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row r="14" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>34</v>
       </c>
@@ -1096,7 +1114,7 @@
         <v>42851237</v>
       </c>
       <c r="E14" s="6">
-        <v>17.67946751063574</v>
+        <v>17.679467510635739</v>
       </c>
       <c r="F14" s="5">
         <v>18936</v>
@@ -1114,7 +1132,7 @@
         <v>21.202664330511997</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row r="15" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1128,7 +1146,7 @@
         <v>58608800</v>
       </c>
       <c r="E15" s="6">
-        <v>2.129588572032574</v>
+        <v>2.1295885720325738</v>
       </c>
       <c r="F15" s="5">
         <v>0</v>
@@ -1143,10 +1161,10 @@
         <v>38751887</v>
       </c>
       <c r="J15" s="6">
-        <v>4.018895980584129</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+        <v>4.0188959805841291</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
@@ -1175,10 +1193,10 @@
         <v>114450945</v>
       </c>
       <c r="J16" s="6">
-        <v>57.21285957363571</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+        <v>57.212859573635711</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>40</v>
       </c>
@@ -1192,7 +1210,7 @@
         <v>117185083</v>
       </c>
       <c r="E17" s="6">
-        <v>76.28142118921079</v>
+        <v>76.281421189210789</v>
       </c>
       <c r="F17" s="5">
         <v>121341</v>
@@ -1207,10 +1225,10 @@
         <v>117116597</v>
       </c>
       <c r="J17" s="6">
-        <v>67.57404752132992</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+        <v>67.574047521329916</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>42</v>
       </c>
@@ -1239,10 +1257,10 @@
         <v>156987698</v>
       </c>
       <c r="J18" s="6">
-        <v>42.51151224517732</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+        <v>42.511512245177322</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>44</v>
       </c>
@@ -1271,10 +1289,10 @@
         <v>156863950</v>
       </c>
       <c r="J19" s="6">
-        <v>4.021950074385358</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+        <v>4.0219500743853578</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
@@ -1306,7 +1324,7 @@
         <v>36.051338085101364</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+    <row r="21" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>48</v>
       </c>
@@ -1320,7 +1338,7 @@
         <v>1806067135</v>
       </c>
       <c r="E21" s="6">
-        <v>55.05600108986101</v>
+        <v>55.056001089861013</v>
       </c>
       <c r="F21" s="5">
         <v>4258252</v>
@@ -1338,7 +1356,7 @@
         <v>48.983863109648304</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+    <row r="22" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
@@ -1352,7 +1370,7 @@
         <v>2063645</v>
       </c>
       <c r="E22" s="6">
-        <v>5.749323697473373</v>
+        <v>11.498647394946746</v>
       </c>
       <c r="F22" s="5">
         <v>333</v>
@@ -1370,7 +1388,7 @@
         <v>17.285699251904553</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+    <row r="23" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>52</v>
       </c>
@@ -1384,7 +1402,7 @@
         <v>4081946</v>
       </c>
       <c r="E23" s="6">
-        <v>8.93484394460411</v>
+        <v>17.869687889208219</v>
       </c>
       <c r="F23" s="5">
         <v>4868</v>
@@ -1402,7 +1420,7 @@
         <v>21.786077493816983</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+    <row r="24" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>54</v>
       </c>
@@ -1416,7 +1434,7 @@
         <v>8029377</v>
       </c>
       <c r="E24" s="6">
-        <v>14.359327580811016</v>
+        <v>28.718655161622031</v>
       </c>
       <c r="F24" s="5">
         <v>21068</v>
@@ -1434,7 +1452,7 @@
         <v>24.424577027661538</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+    <row r="25" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>56</v>
       </c>
@@ -1448,7 +1466,7 @@
         <v>15673919</v>
       </c>
       <c r="E25" s="6">
-        <v>23.7323966907111</v>
+        <v>47.464793381422197</v>
       </c>
       <c r="F25" s="5">
         <v>40184</v>
@@ -1466,7 +1484,7 @@
         <v>31.603244602808637</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
+    <row r="26" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>58</v>
       </c>
@@ -1480,7 +1498,7 @@
         <v>30290104</v>
       </c>
       <c r="E26" s="6">
-        <v>40.117961500663554</v>
+        <v>80.235923001327109</v>
       </c>
       <c r="F26" s="5">
         <v>60416</v>
@@ -1495,10 +1513,10 @@
         <v>30161953</v>
       </c>
       <c r="J26" s="6">
-        <v>40.03783611998799</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
+        <v>40.037836119987993</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>60</v>
       </c>
@@ -1512,7 +1530,7 @@
         <v>57814555</v>
       </c>
       <c r="E27" s="6">
-        <v>69.07057163610645</v>
+        <v>138.1411432722129</v>
       </c>
       <c r="F27" s="5">
         <v>137879</v>
@@ -1527,10 +1545,10 @@
         <v>57706306</v>
       </c>
       <c r="J27" s="6">
-        <v>37.49251978364913</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
+        <v>37.492519783649129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>62</v>
       </c>
@@ -1544,7 +1562,7 @@
         <v>108747344</v>
       </c>
       <c r="E28" s="6">
-        <v>120.22591304828501</v>
+        <v>240.45182609657002</v>
       </c>
       <c r="F28" s="5">
         <v>228316</v>
@@ -1559,10 +1577,10 @@
         <v>108661967</v>
       </c>
       <c r="J28" s="6">
-        <v>41.60502081002537</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
+        <v>41.605020810025373</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>64</v>
       </c>
@@ -1576,7 +1594,7 @@
         <v>201086863</v>
       </c>
       <c r="E29" s="6">
-        <v>210.3441071559326</v>
+        <v>420.68821431186518</v>
       </c>
       <c r="F29" s="5">
         <v>263944</v>
@@ -1591,10 +1609,10 @@
         <v>201023463</v>
       </c>
       <c r="J29" s="6">
-        <v>56.89833037458403</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
+        <v>56.898330374584027</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>66</v>
       </c>
@@ -1608,7 +1626,7 @@
         <v>3521310</v>
       </c>
       <c r="E30" s="6">
-        <v>34.231012258309114</v>
+        <v>68.462024516618229</v>
       </c>
       <c r="F30" s="5">
         <v>9301</v>
@@ -1626,7 +1644,7 @@
         <v>39.355458448524075</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+    <row r="31" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>68</v>
       </c>
@@ -1640,7 +1658,7 @@
         <v>7248722</v>
       </c>
       <c r="E31" s="6">
-        <v>36.26518778673311</v>
+        <v>72.530375573466216</v>
       </c>
       <c r="F31" s="5">
         <v>16521</v>
@@ -1655,10 +1673,10 @@
         <v>7218010</v>
       </c>
       <c r="J31" s="6">
-        <v>42.43101335901619</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
+        <v>42.431013359016191</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>70</v>
       </c>
@@ -1672,7 +1690,7 @@
         <v>14843582</v>
       </c>
       <c r="E32" s="6">
-        <v>38.187071496011136</v>
+        <v>76.374142992022271</v>
       </c>
       <c r="F32" s="5">
         <v>43695</v>
@@ -1690,7 +1708,7 @@
         <v>33.200173288685455</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+    <row r="33" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>72</v>
       </c>
@@ -1704,7 +1722,7 @@
         <v>30290104</v>
       </c>
       <c r="E33" s="6">
-        <v>40.117961500663554</v>
+        <v>80.235923001327109</v>
       </c>
       <c r="F33" s="5">
         <v>60416</v>
@@ -1719,10 +1737,10 @@
         <v>30161953</v>
       </c>
       <c r="J33" s="6">
-        <v>40.03783611998799</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
+        <v>40.037836119987993</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>73</v>
       </c>
@@ -1736,7 +1754,7 @@
         <v>61604169</v>
       </c>
       <c r="E34" s="6">
-        <v>42.034961031588225</v>
+        <v>84.069922063176449</v>
       </c>
       <c r="F34" s="5">
         <v>189948</v>
@@ -1751,10 +1769,10 @@
         <v>61343269</v>
       </c>
       <c r="J34" s="6">
-        <v>29.11979490596407</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
+        <v>29.119794905964071</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>75</v>
       </c>
@@ -1768,7 +1786,7 @@
         <v>124942349</v>
       </c>
       <c r="E35" s="6">
-        <v>43.904167795524415</v>
+        <v>87.808335591048831</v>
       </c>
       <c r="F35" s="5">
         <v>280499</v>
@@ -1783,10 +1801,10 @@
         <v>124412652</v>
       </c>
       <c r="J35" s="6">
-        <v>33.95084787900049</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
+        <v>33.950847879000492</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>77</v>
       </c>
@@ -1800,7 +1818,7 @@
         <v>252819809</v>
       </c>
       <c r="E36" s="6">
-        <v>45.79798530014351</v>
+        <v>91.595970600287018</v>
       </c>
       <c r="F36" s="5">
         <v>403463</v>
@@ -1818,7 +1836,7 @@
         <v>40.424786815060266</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
+    <row r="37" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>79</v>
       </c>
@@ -1832,7 +1850,7 @@
         <v>510588330</v>
       </c>
       <c r="E37" s="6">
-        <v>47.68201198409144</v>
+        <v>95.364023968182877</v>
       </c>
       <c r="F37" s="5">
         <v>1269873</v>
@@ -1851,6 +1869,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>